<commit_message>
Add chatting, Fix multicast bug
</commit_message>
<xml_diff>
--- a/packet model.xlsx
+++ b/packet model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MoonBackSan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MoonBackSan\Desktop\The Vampire Project\The Vampire Server\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="115">
   <si>
     <t>Server</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -271,151 +271,219 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>s [room info]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>71(G)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>room chat R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>102(f)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>room chat (multicast)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[chat]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>72(H)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>room exit R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>103(g)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>73(I)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>104(h)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>74(J)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>105(i)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>75(K)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>106(j)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>107</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>108</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>109</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>110</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>111</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>112</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>113</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>114</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>115</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>116</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>117</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>118</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>88(X)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>119</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>120</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>122(z)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>unknown error</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sign up R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sign up</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[id] [password]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s / f</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[room number]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[101]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[68], [70], [72]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>show friends R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>room update (multicast)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>s [room info]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>config, enter</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>71(G)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>room chat R</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>102(f)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>room chat (multicast)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[chat]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[sender] [chat]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>72(H)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>room exit R</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>103(g)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>room exit</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>73(I)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>104(h)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>74(J)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>105(i)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>75(K)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>106(j)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>107</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>108</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>109</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>110</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>111</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>112</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>113</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>114</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>115</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>116</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>117</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>118</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>88(X)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>119</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>120</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>121</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>122(z)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>unknown error</t>
+    <t>show friends</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add friend</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add friend R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;empty&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[friend id]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[friends list]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f1: add myself</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s / f / f1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>delete friend R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>notice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>121(x)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[sender]\r\n[chat]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>\r\n: separator</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -480,7 +548,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -503,6 +571,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -793,8 +864,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -807,36 +878,36 @@
     <col min="6" max="6" width="23.625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="1.25" customWidth="1"/>
     <col min="8" max="9" width="30.625" customWidth="1"/>
-    <col min="10" max="10" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8" t="s">
+      <c r="I2" s="9"/>
+      <c r="J2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="8"/>
+      <c r="K2" s="9"/>
     </row>
     <row r="3" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8" t="s">
+      <c r="D3" s="9"/>
+      <c r="E3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="8"/>
+      <c r="F3" s="9"/>
       <c r="G3" s="2"/>
       <c r="H3" s="5" t="s">
         <v>1</v>
@@ -1009,117 +1080,141 @@
     <row r="11" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>99</v>
+      </c>
       <c r="E11" s="3" t="s">
         <v>60</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>61</v>
+        <v>101</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>63</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="J11" s="3"/>
       <c r="K11" s="3"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="F12" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="J12" s="3"/>
+        <v>113</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>114</v>
+      </c>
       <c r="K12" s="3"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B13" s="3"/>
       <c r="C13" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>72</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="E13" s="3"/>
       <c r="F13" s="3" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>59</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D14" s="3"/>
+        <v>70</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>93</v>
+      </c>
       <c r="E14" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F14" s="3"/>
+        <v>69</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
+      <c r="H14" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>96</v>
+      </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B15" s="3"/>
       <c r="C15" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D15" s="3"/>
+        <v>72</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>100</v>
+      </c>
       <c r="E15" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="F15" s="3"/>
+        <v>71</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
+      <c r="H15" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D16" s="3"/>
+        <v>74</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>104</v>
+      </c>
       <c r="E16" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F16" s="3"/>
+        <v>73</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>103</v>
+      </c>
       <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
+      <c r="H16" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>108</v>
+      </c>
       <c r="K16" s="3"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.3">
@@ -1127,13 +1222,15 @@
       <c r="C17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3" t="s">
-        <v>80</v>
-      </c>
+      <c r="D17" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
+      <c r="H17" s="3" t="s">
+        <v>106</v>
+      </c>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
@@ -1145,7 +1242,7 @@
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -1161,7 +1258,7 @@
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
@@ -1177,7 +1274,7 @@
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -1193,7 +1290,7 @@
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
@@ -1209,7 +1306,7 @@
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -1225,7 +1322,7 @@
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
@@ -1241,7 +1338,7 @@
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
@@ -1257,7 +1354,7 @@
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
@@ -1273,7 +1370,7 @@
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
@@ -1289,7 +1386,7 @@
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
@@ -1305,7 +1402,7 @@
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
@@ -1317,11 +1414,11 @@
     <row r="29" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B29" s="3"/>
       <c r="C29" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
@@ -1337,7 +1434,7 @@
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
@@ -1353,7 +1450,7 @@
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
@@ -1367,11 +1464,9 @@
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>97</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
       <c r="I32" s="3"/>
@@ -1381,15 +1476,23 @@
     <row r="33" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
+      <c r="E33" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>111</v>
+      </c>
       <c r="G33" s="2"/>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
+      <c r="E34" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>92</v>
+      </c>
       <c r="G34" s="2"/>
     </row>
     <row r="35" spans="3:7" x14ac:dyDescent="0.3">
@@ -1449,10 +1552,10 @@
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="9"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="6"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Add monitoring packet model
</commit_message>
<xml_diff>
--- a/packet model.xlsx
+++ b/packet model.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="123">
   <si>
     <t>Server</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -139,355 +139,383 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>97(a)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>condition</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>login R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>login</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[id] [password]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>66(B)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lobby info R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>98(b)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lobby info</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;empty&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>67(C)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>room create R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>99(c)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>room create</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[maxNum] [isPublic]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[num] [maxNum] [isPublic]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>68(D)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>room config R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[101]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>69(E)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>specific room enter R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>100(d)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fail to enter</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[room number]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>70(F)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>room enter R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[101]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;empty&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>101(e)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>71(G)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>room chat R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>102(f)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>room chat (multicast)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>72(H)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>room exit R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>103(g)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>73(I)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>104(h)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>74(J)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>105(i)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>75(K)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>106(j)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>107</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>108</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>109</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>110</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>111</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>112</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>113</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>114</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>115</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>116</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>122(z)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>unknown error</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sign up R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sign up</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[id] [password]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s / f</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[room number]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[101]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[68], [70], [72]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>show friends R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>room update (multicast)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>show friends</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add friend</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add friend R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;empty&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[friend id]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[friends list]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f1: add myself</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s / f / f1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>delete friend R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>notice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>\r\n: separator</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s [room info] / f</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f: room unabled</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>88(X)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>117</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>118</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>119</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[infomation of server]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>a(ll) / r(ooms) / c(lients) / e(rrors)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>89(Y)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>90(Z)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>97(a)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>condition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>login R</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>login</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[id] [password]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>X</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>66(B)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>lobby info R</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>98(b)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>lobby info</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;empty&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>67(C)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>room create R</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>99(c)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>room create</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[maxNum] [isPublic]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[num] [maxNum] [isPublic]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>68(D)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>room config R</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[101]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>69(E)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>specific room enter R</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>100(d)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fail to enter</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[room number]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>f</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>70(F)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>room enter R</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[101]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;empty&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>101(e)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>71(G)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>room chat R</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>102(f)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>room chat (multicast)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[chat]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>72(H)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>room exit R</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>103(g)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>73(I)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>104(h)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>74(J)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>105(i)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>75(K)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>106(j)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>107</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>108</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>109</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>110</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>111</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>112</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>113</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>114</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>115</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>116</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>117</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>118</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>88(X)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>119</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>120</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>122(z)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>unknown error</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sign up R</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sign up</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[id] [password]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s / f</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[room number]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[101]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[68], [70], [72]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>show friends R</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>room update (multicast)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>show friends</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>add friend</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>add friend R</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;empty&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[friend id]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[friends list]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>f1: add myself</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s / f / f1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>delete friend R</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>notice</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>121(x)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[sender]\r\n[chat]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>\r\n: separator</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>s [room info] / f</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>f: room unabled</t>
+    <t>89(Z)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>120(x)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>121(y)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>notice R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>by admin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[notice type] [message]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[message]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[sender]\r\n[message]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>monitor R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>monitor</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -552,7 +580,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -575,9 +603,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -868,8 +893,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -887,31 +912,31 @@
   <sheetData>
     <row r="1" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
       <c r="G2" s="2"/>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9" t="s">
+      <c r="I2" s="8"/>
+      <c r="J2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="K2" s="9"/>
+      <c r="K2" s="8"/>
     </row>
     <row r="3" spans="2:11" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="9"/>
+      <c r="F3" s="8"/>
       <c r="G3" s="2"/>
       <c r="H3" s="5" t="s">
         <v>1</v>
@@ -920,7 +945,7 @@
         <v>9</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="2:11" ht="17.25" x14ac:dyDescent="0.3">
@@ -949,17 +974,17 @@
         <v>8</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I5" s="3" t="s">
         <v>11</v>
@@ -969,23 +994,23 @@
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="I6" s="3" t="s">
         <v>12</v>
@@ -996,23 +1021,23 @@
     <row r="7" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -1020,18 +1045,18 @@
     <row r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" s="3"/>
       <c r="C8" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
@@ -1040,23 +1065,23 @@
     <row r="9" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B9" s="3"/>
       <c r="C9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
@@ -1064,18 +1089,18 @@
     <row r="10" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B10" s="3"/>
       <c r="C10" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
@@ -1085,65 +1110,65 @@
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="K11" s="3"/>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B12" s="3"/>
       <c r="C12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="F12" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3" t="s">
-        <v>65</v>
+        <v>119</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="K12" s="3"/>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B13" s="3"/>
       <c r="C13" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
@@ -1152,23 +1177,23 @@
     <row r="14" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B14" s="3"/>
       <c r="C14" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -1176,23 +1201,23 @@
     <row r="15" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B15" s="3"/>
       <c r="C15" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
@@ -1200,26 +1225,26 @@
     <row r="16" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B16" s="3"/>
       <c r="C16" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="K16" s="3"/>
     </row>
@@ -1229,13 +1254,13 @@
         <v>16</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
@@ -1248,7 +1273,7 @@
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
@@ -1264,7 +1289,7 @@
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
@@ -1280,7 +1305,7 @@
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
@@ -1296,7 +1321,7 @@
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
@@ -1312,7 +1337,7 @@
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
@@ -1328,7 +1353,7 @@
       </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
@@ -1344,7 +1369,7 @@
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
@@ -1360,7 +1385,7 @@
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
@@ -1376,7 +1401,7 @@
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
@@ -1392,7 +1417,7 @@
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
@@ -1408,7 +1433,7 @@
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
@@ -1420,11 +1445,11 @@
     <row r="29" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B29" s="3"/>
       <c r="C29" s="3" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3" t="s">
-        <v>85</v>
+        <v>107</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
@@ -1435,12 +1460,10 @@
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B30" s="3"/>
-      <c r="C30" s="3" t="s">
-        <v>28</v>
-      </c>
+      <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3" t="s">
-        <v>86</v>
+        <v>108</v>
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
@@ -1451,12 +1474,10 @@
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B31" s="3"/>
-      <c r="C31" s="3" t="s">
-        <v>29</v>
-      </c>
+      <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3" t="s">
-        <v>88</v>
+        <v>109</v>
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
@@ -1467,55 +1488,86 @@
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="3"/>
+      <c r="C32" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>121</v>
+      </c>
       <c r="E32" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="F32" s="3"/>
+        <v>114</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>122</v>
+      </c>
       <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
+      <c r="H32" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>117</v>
+      </c>
       <c r="K32" s="3"/>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
+    <row r="33" spans="3:10" x14ac:dyDescent="0.3">
+      <c r="C33" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>116</v>
+      </c>
       <c r="E33" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="F33" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="G33" s="2"/>
-    </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.3">
+        <v>115</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="34" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="G34" s="2"/>
-    </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+    </row>
+    <row r="35" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
-      <c r="G35" s="2"/>
-    </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+    </row>
+    <row r="36" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="G36" s="2"/>
     </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:10" x14ac:dyDescent="0.3">
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
@@ -1558,10 +1610,10 @@
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="10"/>
+      <c r="C4" s="9"/>
       <c r="D4" s="6"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">

</xml_diff>